<commit_message>
- Aider: mis à jour les procédures. - Doc: mis à jour la liste des modules.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@21461 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Resources/Module list.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Resources/Module list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="42195" windowHeight="23040"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -93,12 +93,6 @@
     <t>Crésus Graphe</t>
   </si>
   <si>
-    <t>Cresus.Assets</t>
-  </si>
-  <si>
-    <t>Crésus Immobilisations</t>
-  </si>
-  <si>
     <t>Cresus.WebServer</t>
   </si>
   <si>
@@ -111,17 +105,62 @@
     <t>composant serveur web</t>
   </si>
   <si>
-    <t>Projet "AIDER" de l'EERV</t>
-  </si>
-  <si>
-    <t>Product.Aider</t>
+    <t>Core.Library.Data</t>
+  </si>
+  <si>
+    <t>Core.Library</t>
+  </si>
+  <si>
+    <t>Core.Library.Address</t>
+  </si>
+  <si>
+    <t>Core.Library.Documents</t>
+  </si>
+  <si>
+    <t>Core.Library.Features</t>
+  </si>
+  <si>
+    <t>Core.Library.Finance</t>
+  </si>
+  <si>
+    <t>Core.Library.Images</t>
+  </si>
+  <si>
+    <t>Core.Library.Measures</t>
+  </si>
+  <si>
+    <t>Core.Library.UI</t>
+  </si>
+  <si>
+    <t>Core.Library.UserManagement</t>
+  </si>
+  <si>
+    <t>Core.Library.Workflows</t>
+  </si>
+  <si>
+    <t>Core.Library.Business</t>
+  </si>
+  <si>
+    <t>Data.Platform.SwissPostMatch</t>
+  </si>
+  <si>
+    <t>Aider</t>
+  </si>
+  <si>
+    <t>Produit "AIDER" développé pour l'EERV</t>
+  </si>
+  <si>
+    <t>Product.Assets.Data</t>
+  </si>
+  <si>
+    <t>Cresus.Compta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +170,14 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,11 +204,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +646,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,7 +660,7 @@
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -623,13 +671,13 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -690,44 +738,195 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>1001</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1002</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>1003</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>1004</v>
       </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" t="s">
-        <v>26</v>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1005</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1006</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>1007</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1008</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1009</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1010</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1011</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1012</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>1013</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1014</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1016</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>2000</v>
       </c>
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" t="s">
         <v>23</v>
-      </c>
-      <c r="D38" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- AIDER: mise à jour des lignes de commandes. - Doc: liste des modules (ressources) mise à jour.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@23574 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Resources/Module list.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Resources/Module list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -150,10 +150,25 @@
     <t>Produit "AIDER" développé pour l'EERV</t>
   </si>
   <si>
-    <t>Product.Assets.Data</t>
-  </si>
-  <si>
     <t>Cresus.Compta</t>
+  </si>
+  <si>
+    <t>Assets.Server</t>
+  </si>
+  <si>
+    <t>Assets.Server.Engine</t>
+  </si>
+  <si>
+    <t>Assets.Server.DataFillers</t>
+  </si>
+  <si>
+    <t>Assets.Data</t>
+  </si>
+  <si>
+    <t>Assets.Core</t>
+  </si>
+  <si>
+    <t>Assets.App</t>
   </si>
 </sst>
 </file>
@@ -206,10 +221,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,12 +541,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -770,16 +785,16 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>1003</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -883,16 +898,16 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>1013</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -912,7 +927,7 @@
         <v>1016</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
         <v>23</v>
@@ -923,9 +938,64 @@
         <v>2000</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2001</v>
+      </c>
+      <c r="B52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2002</v>
+      </c>
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2003</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2004</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2005</v>
+      </c>
+      <c r="B56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assets: ajouté un fichier de ressources pour Server.Export.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Resources/Module list.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Resources/Module list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Assets.App</t>
+  </si>
+  <si>
+    <t>Assets.Server.Export</t>
   </si>
 </sst>
 </file>
@@ -526,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,6 +999,17 @@
         <v>46</v>
       </c>
       <c r="C56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2006</v>
+      </c>
+      <c r="B57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>